<commit_message>
completed xpaths and column a
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Update_Reporting/artifacts/service_model/information_model/IEPD/documentation/Hawaii JJIS to CCH.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Criminal_History_Update_Reporting/artifacts/service_model/information_model/IEPD/documentation/Hawaii JJIS to CCH.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haiqiwei/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/celeste/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44336C38-73AD-4848-B816-A3BA3F74C040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E013DB2-A29F-1F42-A680-556C4C8F6A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="40960" windowHeight="22540" xr2:uid="{005F782A-DF2E-4A52-944D-3DDF0FF535F1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{005F782A-DF2E-4A52-944D-3DDF0FF535F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Prosecutor Dispos LEIN CCH" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="429">
   <si>
     <t>Fingerprint Transaction Control Number</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>State Identification number</t>
-  </si>
-  <si>
-    <t>CTN</t>
   </si>
   <si>
     <t>Criminal Tracking Number</t>
@@ -334,6 +331,1032 @@
   </si>
   <si>
     <t>Hawaii Juvenile Justice System Mapping Spread Sheet</t>
+  </si>
+  <si>
+    <t>/exc:JJISProsCaseExchange/j:Case/nc:CaseTrackingID</t>
+  </si>
+  <si>
+    <t>tblCsCases.fileNumber</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>/pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestAgency/nc:OrganizationIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>Location: /exc:JJISProsCaseExchange/j:Case/nc:CaseFiling/nc:DocumentSubmitter/nc:EntityOrganization/nc:OrganizationIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>&lt;!-- FIXED 31 for all for Charge Screen, Referral Tab, Agency, "Hawaii Police Department"--&gt;</t>
+  </si>
+  <si>
+    <t>Location: /exc:JJISProsCaseExchange/j:Case/nc:CaseFiling/nc:DocumentSubmitter/nc:EntityOrganization/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>Location: /pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>&lt;!-- for Charge Screen, Referral Tab, Agency, "Hawaii Police Department" --&gt;</t>
+  </si>
+  <si>
+    <t>Location: /exc:JJISProsCaseExchange/j:Case/nc:CaseFiling/nc:DocumentReceivedDate/nc:Date</t>
+  </si>
+  <si>
+    <t>Location: /pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Case/nc:CaseFiling/nc:DocumentFiledDate/nc:Date</t>
+  </si>
+  <si>
+    <t>tblCsDocument.CreateDate</t>
+  </si>
+  <si>
+    <t>Location: /pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeApplicabilityText</t>
+  </si>
+  <si>
+    <t>Location: /exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge[1]/j:ChargeApplicabilityText</t>
+  </si>
+  <si>
+    <t>Location: /pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeCountQuantity</t>
+  </si>
+  <si>
+    <t>Location: /exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge[1]/j:ChargeCountQuantity</t>
+  </si>
+  <si>
+    <t>&lt;!--tblCsCharge.CountNumber (SO GM ChargeCountQuantity vs ChargeSequenceID?) tblCsCharge.count, Charge Tab, "#" column (1, 2, 3 etc) --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- SO GM, JJIS parse Charge modifier from (HcPA has charge codes that include the modifiers) --&gt;</t>
+  </si>
+  <si>
+    <t>Location: /pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeDescriptionText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tblCsCharge.chargeDescription </t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeDisposition/nc:DispositionDate/nc:Date</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeDisposition/nc:DispositionDate/nc:Date</t>
+  </si>
+  <si>
+    <t>tblCsCharge.dispositionDate</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeDisposition/nc:DispositionDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeDisposition/nc:DispositionDescriptionText</t>
+  </si>
+  <si>
+    <t>tblCtEventCodes.DispositionCodeDescription</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeDisposition/nc:DispositionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeDisposition/nc:DispositionText</t>
+  </si>
+  <si>
+    <t>tblCsCharge.DispositionCode</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeSequenceID/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>tblCsCharge.ChargeCodeSequence</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>&lt;!-- 4058 for 702-221(2)(c) &amp; 702-222(1)(b) &amp; 705-500 &amp; 707-701(1)(a), Accomplice to Attempted Murder in the First Degree, Line 6474 in State Charges xls --&gt;</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeSequenceID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">					&lt;!--tblCsCharge.CountNumber, Charge Tab, "#" column (1, 2, 3 etc) in Karpel --&gt;&lt;!--SO GM ChargeCountQuantity vs ChargeSequenceID? tblCsCharge.count OR tblCsCharge.sequenceID? --&gt;</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeSeverityText</t>
+  </si>
+  <si>
+    <t>&lt;!-- tblCsCharge.severity concat with tblCsCharge.Class, Charge screen, GREEN Under "Desc" look for "Severity" --&gt;</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeSeverityLevel/j:SeverityLevelDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Arrest/j:ArrestCharge/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeStatute/j:StatuteCodeSectionIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>&lt;!--tblCsCharge.chargeCode- Charge screen, click on Statute, Green box on right right of Charge screen, I.e. 708-833(1)-10 from CODE column in StateChargeCode.XLS --&gt;</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Offense/j:OffenseViolatedStatute/j:StatuteDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeStatute/j:StatuteDescriptionText</t>
+  </si>
+  <si>
+    <t>tblCsCharge.chargeDescription</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Offense/j:OffenseViolatedStatute/j:StatuteLevelText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeStatute/j:StatuteLevelText</t>
+  </si>
+  <si>
+    <t>tblCsCharge.severity</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Offense/j:OffenseViolatedStatute/j:StatuteCodeSectionIdentification/nc:IdentificationJurisdictionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeTrackingIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeTrackingIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>tblCsCharge.policeReportNo</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeApplicabilityText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeStatute/j:StatuteCodeIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeStatute/j:StatuteCodeSectionIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeStatute/j:StatuteDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeStatute/j:StatuteLevelText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeSeverityLevel/j:SeverityLevelDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeSequenceID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeDisposition/nc:DispositionDate/nc:Date</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeDisposition/nc:DispositionDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeDisposition/nc:DispositionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeCountQuantity</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeDegreeText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Charge/j:ChargeCountQuantity</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeApplicabilityText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonAlternateName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonAlternateName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonAlternateName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonAlternateName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonAlternateName/nc:PersonNameSuffixText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonAlternateName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonAlternateName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonAlternateName/nc:PersonNameSuffixText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonAlternateName/nc:AliasIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonAlternateName/ext:PersonAlternateNameIdnt/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonAlternateName/nc:AliasIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonAlternateName/ext:PersonAlternateNameIdnt/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonEthnicityText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/j:PersonEyeColorCode</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonEyeColorText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/j:PersonHairColorCode</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonHairColorText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonEthnicityText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonEyeColorCode</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonEyeColorText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonHairColorCode</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonHairColorText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonHeightMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonHeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonHeightMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonHeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonName/nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonName/nc:PersonFullName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonOtherIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonOtherIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonOtherIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonOtherIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureGeneralCategoryText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureCategoryCode</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureCategoryText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureLocationText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonPhysicalFeature/nc:PhysicalFeatureIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonPhysicalFeature/nc:PhysicalFeatureGeneralCategoryText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonPhysicalFeature/nc:PhysicalFeatureCategoryCode</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonPhysicalFeature/nc:PhysicalFeatureCategoryText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonPhysicalFeature/nc:PhysicalFeatureDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonPhysicalFeature/nc:PhysicalFeatureLocationText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonPhysicalFeature/ext:PersonPhysicalFeatureIdnt/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/ext:PersonPhysicalFeature/ext:PersonPhysicalFeatureIdnt/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/j:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonResidentText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonSSNIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonUSCitizenIndicator</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonWeightMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Person/nc:PersonWeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonRaceText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonSexCode</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonSexText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonWeightMeasure/nc:MeasureValueText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Person/nc:PersonWeightMeasure/nc:MeasureUnitText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:ContactInformation/nc:ContactWebsiteURI</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:ContactInformation/nc:ContactTelephoneNumber</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:ContactInformation/nc:ContactMobileTelephoneNumber/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:ContactInformation/nc:ContactMobileTelephoneNumber/nc:FullTelephoneNumber/nc:TelephoneSuffixID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:ContactInformation/nc:ContactEntityDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:ContactInformation/nc:ContactMobileTelephoneNumber/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:ContactInformation/nc:ContactEntityDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc:AddressSecondaryUnitText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc:LocationStateName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:Address/nc:LocationPostalExtensionCode</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/nc:LocationAddress/nc:StructuredAddress/nc:AddressSecondaryUnitText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationStateName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/nc:LocationAddress/nc:StructuredAddress/nc:LocationPostalExtensionCode</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:LocationCategoryText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:LocationContactInformation/nc:ContactTelephoneNumber/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:LocationContactInformation/nc:ContactTelephoneNumber/nc:FullTelephoneNumber/nc:TelephoneSuffixID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:LocationContactInformation/nc:ContactEntityDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/nc:LocationCategoryText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/nc:LocationContactInformation/nc:ContactTelephoneNumber/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/nc:LocationContactInformation/nc:ContactEntityDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:LocationIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:LocationIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Location/nc:LocationIdentification/nc:IdentificationEffectiveDate/nc:Date</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/ext:LocationIdnt/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/ext:LocationIdnt/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/ext:Location/ext:LocationIdnt/nc:IdentificationEffectiveDate/nc:Date</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Offense/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Offense/nc:ActivityIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Offense/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:Offense/j:OffenseViolatedStatute/j:StatuteCodeSectionIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Offense/nc:ActivityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Offense/nc:ActivityIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Offense/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Offense/j:OffenseViolatedStatute/j:StatuteCodeSectionIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Offense/j:OffenseViolatedStatute/j:StatuteCodeSectionIdentification/nc:IdentificationJurisdictionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Offense/j:OffenseViolatedStatute/j:StatuteDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:Offense/j:OffenseViolatedStatute/j:StatuteLevelText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationAbbreviationText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationCategoryText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:Address/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:Address/nc:AddressSecondaryUnitText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:Address/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:Address/nc:LocationStateName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:Address/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:Address/nc:LocationPostalExtensionCode</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:LocationCategoryText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:LocationContactInformation/nc:ContactTelephoneNumber/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:LocationContactInformation/nc:ContactTelephoneNumber/nc:FullTelephoneNumber/nc:TelephoneSuffixID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:LocationContactInformation/nc:ContactEntityDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:LocationIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationLocation/nc:LocationIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:Organization/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/nc:OrganizationAbbreviationText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/nc:OrganizationCategoryText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/nc:OrganizationIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/nc:OrganizationIdentification/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/ext:OrganizationLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationStreet/nc:StreetFullText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/ext:OrganizationLocation/nc:LocationAddress/nc:StructuredAddress/nc:AddressSecondaryUnitText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/ext:OrganizationLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationCityName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/ext:OrganizationLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationStateName</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/ext:OrganizationLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationPostalCode</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/ext:OrganizationLocation/nc:LocationAddress/nc:StructuredAddress/nc:LocationPostalExtensionCode</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/ext:OrganizationLocation/nc:LocationCategoryText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/ext:OrganizationLocation/nc:LocationContactInformation/nc:ContactTelephoneNumber/nc:FullTelephoneNumber/nc:TelephoneNumberFullID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/ext:OrganizationLocation/ext:LocationIdnt/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/ext:OrganizationLocation/ext:LocationIdnt/nc:IdentificationCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:Organization/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:CohabitantAssociation/nc:AssociationDateRange/nc:StartDate/nc:Date</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:CohabitantAssociation/nc:AssociationDateRange/nc:EndDate/nc:Date</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:CohabitantAssociation/nc:Person</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:CohabitantAssociation/nc:AssociationBeginDate/nc:Date</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:CohabitantAssociation/nc:PersonReference</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:ImmediateFamilyAssociation/nc:Parent</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:ImmediateFamilyAssociation/nc:Child</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:ImmediateFamilyAssociation/nc:FamilyKinshipText</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:ImmediateFamilyAssociation/nc:PersonParentReference</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:ImmediateFamilyAssociation/nc:PersonChildReference</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:ImmediateFamilyAssociation/nc:FamilyKinshipText</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:OffenseChargeAssociation/j:Offense</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:OffenseChargeAssociation/j:OffenseReference</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:OffenseChargeAssociation/j:Charge</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:OffenseChargeAssociation/j:ChargeReference</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:OffenseLocationAssociation/j:Offense</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:OffenseLocationAssociation/nc:Location</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:OffenseLocationAssociation/j:OffenseReference</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:OffenseLocationAssociation/nc:LocationReference</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:OffenseSubjectAssociation/j:Offense</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:OffenseSubjectAssociation/j:Subject/nc:RoleOfPerson</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:OffenseSubjectAssociation/j:OffenseJuvenileIndicator</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/j:OffenseSubjectAssociation/j:OffenseUnderInfluenceIndicator</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:OffenseSubjectAssociation/j:OffenseReference</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:OffenseSubjectAssociation/j:SubjectReference</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/j:OffenseSubjectAssociation/j:OffenseJuvenileIndicator</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonContactInformationAssociation/nc:AssociationDateRange/nc:StartDate/nc:Date</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonContactInformationAssociation/nc:AssociationDateRange/nc:EndDate/nc:Date</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonContactInformationAssociation/nc:Person</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonContactInformationAssociation/nc:ContactInformation</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonContactInformationAssociation/nc:ContactInformationIsPrimaryIndicator</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonContactInformationAssociation/nc:ContactInformationIsHomeIndicator</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonContactInformationAssociation/nc:ContactInformationIsWorkIndicator</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:PersonContactInformationAssociation/nc:AssociationBeginDate/nc:Date</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:PersonContactInformationAssociation/nc:PersonReference</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:PersonContactInformationAssociation/nc:ContactInformationReference</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:PersonContactInformationAssociation/nc:ContactInformationIsPrimaryIndicator</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:PersonContactInformationAssociation/nc:ContactInformationIsHomeIndicator</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:PersonContactInformationAssociation/nc:ContactInformationIsWorkIndicator</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonOrganizationAssociation/nc:Person</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonOrganizationAssociation/nc:Organization</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:PersonOrganizationAssociation/nc:PersonReference</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:PersonOrganizationAssociation/nc:OrganizationReference</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonResidenceAssociation/nc:AssociationDateRange/nc:StartDate/nc:Date</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonResidenceAssociation/nc:AssociationDateRange/nc:EndDate/nc:Date</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonResidenceAssociation/nc:Person</t>
+  </si>
+  <si>
+    <t>pdr-report-doc:ProsecutionDecisionRecordingReport/nc:PersonResidenceAssociation/nc:Location</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:ResidenceAssociation/nc:AssociationBeginDate/nc:Date</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:ResidenceAssociation/nc:PersonReference</t>
+  </si>
+  <si>
+    <t>exc:JJISProsCaseExchange/nc:ResidenceAssociation/nc:LocationReference</t>
+  </si>
+  <si>
+    <t>&lt;!-- Line 6474 in State Charges xls--&gt;</t>
+  </si>
+  <si>
+    <t>tblCsCharge.CountNumber</t>
+  </si>
+  <si>
+    <t>tblCsCharge.chargeCode</t>
+  </si>
+  <si>
+    <t>tblDfAliasHistory.FirstName</t>
+  </si>
+  <si>
+    <t>tblDfAliasHistory.FirstMiddle</t>
+  </si>
+  <si>
+    <t>tblDfAliasHistory.FirstLast</t>
+  </si>
+  <si>
+    <t>tblDfAliasHistory.NameSuffix</t>
+  </si>
+  <si>
+    <t>tbldfAliasHistory.SequenceNumber</t>
+  </si>
+  <si>
+    <t>&lt;!-- Fixed Text "INTERNAL" --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.Dob</t>
+  </si>
+  <si>
+    <t>tblCtPersonReportingTypes.Description</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.Race 		&lt;!--tblCtRace.Description Person screen, text from "Race" box --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.EyeColor</t>
+  </si>
+  <si>
+    <t>&lt;!--tblCtEyeColor.Description Person screen, text from "Eye" color box --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.HairColor</t>
+  </si>
+  <si>
+    <t>&lt;!--tblCtHairColor.Description Person screen, text from "Hair" color box --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.Height</t>
+  </si>
+  <si>
+    <t>&lt;!--JJIS to translate to FT or IN. Person screen will have 508 in Height box --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.FirstName</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.MiddleName</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.LastName</t>
+  </si>
+  <si>
+    <t>&lt;!--Concatenate with name parts LASTNAME, FIRSTNAME MIDDLENAME Suffix (Ie. JR) --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.DefendantNumber</t>
+  </si>
+  <si>
+    <t>&lt;!-- FIXED Text "INTERNAL"--&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- 5/21/2025- Karpel does NOT have Tatoos --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- ? Not sure what this is --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- GM and SO ? each Person Physical Feature block should have an Id assigned in the back end --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- Fixed "INTERNAL" --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!--Person screen, Gender from "Sex" dropdown --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.Sex</t>
+  </si>
+  <si>
+    <t>&lt;!-- 5/21/2025- Karpel screens do NOT have US Citizen Y/N --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.Weight</t>
+  </si>
+  <si>
+    <t>&lt;!-- "LBS" for weight in pounds --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- tblDfContactInfoPhone.Phone, tblDfContactInfoPhone.Description "Primary", Person screen, Entity "Phone" box--&gt;</t>
+  </si>
+  <si>
+    <t>tblDfContactInfoPhone.Extension</t>
+  </si>
+  <si>
+    <t>&lt;!-- Fixed text description of contact information --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.StreetAddress1</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.StreetAddress2</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.City</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.State</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.ZipCode</t>
+  </si>
+  <si>
+    <t>&lt;!--parse out from tblDfDefendantsWitnesses.ZipCode, Person screen, parse out Postal Extension from "Zip" block --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfContactInfo.Description</t>
+  </si>
+  <si>
+    <t>tblDfContactInfoPhone.Phone</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.Extension</t>
+  </si>
+  <si>
+    <t>&lt;!--TblDfDefendantsWitnesses using the Defendant Number from the tblDfRelations table for PARENT. , Person screen "Entity" box? --&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tblDfDefendantsWitnesses.LocationUniqueIdnt </t>
+  </si>
+  <si>
+    <t>&lt;!-- Fixed text INTERNAL --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfDefendantsWitnesses.UpdateDate</t>
+  </si>
+  <si>
+    <t>&lt;!-- tblCsCharge.TicketNumber Charge screen "C#" above Referral Charges RED/Left side--&gt;</t>
+  </si>
+  <si>
+    <t>tblCsCases.ArrestDate</t>
+  </si>
+  <si>
+    <t>tblCsCharge.ReferredCharge</t>
+  </si>
+  <si>
+    <t>tblCsCharge.JurisdictionCode</t>
+  </si>
+  <si>
+    <t>tblCsCharge.ReferralChargeDescription</t>
+  </si>
+  <si>
+    <t>tblCsCharge.ReferralSeverity</t>
+  </si>
+  <si>
+    <t>tblCtSchool.code</t>
+  </si>
+  <si>
+    <t>&lt;!-- "SCHOOL" if Karpel has Juv School information --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfSchoolEmployAttending.SchoolEmployCode</t>
+  </si>
+  <si>
+    <t>tblCtSchoolEmploy.Description</t>
+  </si>
+  <si>
+    <t>tblCtSchoolEmploy.AddressLine1</t>
+  </si>
+  <si>
+    <t>tblCtSchoolEmploy.City</t>
+  </si>
+  <si>
+    <t>tblCtSchoolEmploy.State</t>
+  </si>
+  <si>
+    <t>tblCtSchoolEmploy.ZipCode</t>
+  </si>
+  <si>
+    <t>&lt;!-- Parse from tblCtSchoolEmploy.ZipCode Person screen, click on "Schools" button, under "Location" column --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- "SCHOOL" for School Info Karpel, Person screen, Schools button, "School/Employment" screen --&gt;</t>
+  </si>
+  <si>
+    <t>tblCtSchoolEmploy.Phone</t>
+  </si>
+  <si>
+    <t>&lt;!-- Parse from tblCtSchoolEmploy.Phone, Karpel Contact Info screen under "Ext" --&gt;</t>
+  </si>
+  <si>
+    <t>tblDfRelations.EnterDate</t>
+  </si>
+  <si>
+    <t>&lt;!-- These reference that idPER004 and idPER001 are associated to each other --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!--tblDfRelations.RelationCode and tblCtRelations.Code FAT for FATHER, Karpel Person screen "Relation" button, "Relation" dropdown or "Person Type" dropdown in "Relation Search" screen--&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- These reference that idPER003 and idPER001 are associated to each other --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- tbldfreportingtype=JO for Juvenile, 0=not juv, 1=juv --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- tblDfDefendantWitness.ReportingType, tblDfReportingType connection is made and tblCtCaseReportingTypes where the types are defined--&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- Karpel, Contact Info screen, "Phone Numbers", "Primary" Y/N --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- Karpel, Contact Info screen, "Resides With" block --&gt;</t>
+  </si>
+  <si>
+    <t>&lt;!-- Karpel, I don't see an example to indicate if contact info is "work" Y/N --&gt;</t>
   </si>
 </sst>
 </file>
@@ -370,7 +1393,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +1403,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,7 +1525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -552,24 +1581,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -582,9 +1593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -593,6 +1601,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -908,15 +1943,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3626C4AD-8C98-4738-B595-8911E3803DFF}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E184"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B131" zoomScale="159" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="23" customWidth="1"/>
+    <col min="1" max="1" width="50.83203125" style="31" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" style="11" customWidth="1"/>
     <col min="3" max="4" width="50.5" style="11" customWidth="1"/>
     <col min="5" max="5" width="68.83203125" style="11" bestFit="1" customWidth="1"/>
@@ -924,306 +1959,2063 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
+      <c r="A1" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" s="13" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>86</v>
+      <c r="A2" s="26" t="s">
+        <v>85</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="E2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="13" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" s="15"/>
+        <v>82</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>89</v>
+      </c>
       <c r="E3" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="13" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D4" s="15"/>
+        <v>69</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>89</v>
+      </c>
       <c r="E4" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="84" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>27</v>
+      <c r="A5" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>89</v>
+      </c>
       <c r="E5" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>89</v>
+      </c>
       <c r="E6" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="70" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="29" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="9" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="8" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="29" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>89</v>
+      </c>
       <c r="E8" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="10" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="29"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="29"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="D28" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="D29" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="D30" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="D31" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="D32" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="11"/>
+      <c r="B33" s="2"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="D34" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="D35" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="D36" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="D37" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="D38" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="32" t="s">
+        <v>357</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="D39" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="32" t="s">
+        <v>358</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="D40" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="32" t="s">
+        <v>359</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="D41" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="D42" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="32" t="s">
+        <v>361</v>
+      </c>
+      <c r="B43" s="2"/>
+      <c r="D43" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="D44" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="32" t="s">
+        <v>363</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="D45" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="B46" s="2"/>
+      <c r="D46" s="34" t="s">
+        <v>178</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="32" t="s">
+        <v>365</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="D47" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="32" t="s">
+        <v>366</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="D48" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="D49" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="32" t="s">
+        <v>368</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="D50" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="32" t="s">
+        <v>369</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="D51" s="34" t="s">
+        <v>185</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="32" t="s">
+        <v>370</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="D52" s="34" t="s">
+        <v>186</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="32" t="s">
+        <v>371</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="D53" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="32" t="s">
+        <v>372</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="D54" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="D55" s="34" t="s">
+        <v>193</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="D56" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="32" t="s">
+        <v>375</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="D57" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="32" t="s">
+        <v>376</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="D58" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="32" t="s">
+        <v>377</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="D59" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="32" t="s">
+        <v>377</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="D60" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="32" t="s">
+        <v>378</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="D61" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="32" t="s">
+        <v>377</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="D62" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="32" t="s">
+        <v>377</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="D63" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="32" t="s">
+        <v>379</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="D64" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="32" t="s">
+        <v>380</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="D65" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="D66" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="32" t="s">
+        <v>364</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="D67" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="11"/>
+      <c r="B68" s="2"/>
+      <c r="E68" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="32" t="s">
+        <v>382</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="D69" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="32" t="s">
+        <v>381</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="D70" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="32"/>
+      <c r="B71" s="2"/>
+      <c r="E71" s="9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="32" t="s">
+        <v>384</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="D73" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="32" t="s">
+        <v>385</v>
+      </c>
+      <c r="B74" s="2"/>
+      <c r="D74" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="32"/>
+      <c r="B75" s="2"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="32"/>
+      <c r="B76" s="2"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="32" t="s">
+        <v>386</v>
+      </c>
+      <c r="B77" s="2"/>
+      <c r="D77" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="32" t="s">
+        <v>388</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="D79" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="32" t="s">
+        <v>389</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="D80" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="B81" s="2"/>
+      <c r="D81" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="32" t="s">
+        <v>391</v>
+      </c>
+      <c r="B82" s="2"/>
+      <c r="D82" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="32" t="s">
+        <v>392</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="D83" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="32" t="s">
+        <v>393</v>
+      </c>
+      <c r="B84" s="2"/>
+      <c r="D84" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="32" t="s">
+        <v>394</v>
+      </c>
+      <c r="B85" s="2"/>
+      <c r="D85" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="D86" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="32" t="s">
+        <v>396</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="D87" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="32" t="s">
+        <v>397</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="D88" s="34"/>
+      <c r="E88" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="32" t="s">
+        <v>398</v>
+      </c>
+      <c r="B89" s="2"/>
+      <c r="D89" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="32" t="s">
+        <v>399</v>
+      </c>
+      <c r="B90" s="2"/>
+      <c r="D90" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="D91" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="32" t="s">
+        <v>401</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="D92" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="B93" s="2"/>
+      <c r="D93" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="32"/>
+      <c r="B94" s="2"/>
+      <c r="D94" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="B95" s="2"/>
+      <c r="D95" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="32" t="s">
+        <v>404</v>
+      </c>
+      <c r="B96" s="2"/>
+      <c r="D96" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="32" t="s">
+        <v>405</v>
+      </c>
+      <c r="B97" s="2"/>
+      <c r="D97" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="B98" s="2"/>
+      <c r="D98" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="32" t="s">
+        <v>407</v>
+      </c>
+      <c r="B99" s="2"/>
+      <c r="D99" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="32" t="s">
+        <v>408</v>
+      </c>
+      <c r="B100" s="2"/>
+      <c r="D100" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="32" t="s">
+        <v>409</v>
+      </c>
+      <c r="B101" s="2"/>
+      <c r="D101" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="B102" s="2"/>
+      <c r="D102" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="32" t="s">
+        <v>411</v>
+      </c>
+      <c r="B103" s="2"/>
+      <c r="D103" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="32" t="s">
+        <v>412</v>
+      </c>
+      <c r="B104" s="2"/>
+      <c r="D104" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="32"/>
+      <c r="B105" s="2"/>
+      <c r="D105" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="B106" s="2"/>
+      <c r="D106" s="34" t="s">
+        <v>294</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="32" t="s">
+        <v>414</v>
+      </c>
+      <c r="B107" s="2"/>
+      <c r="D107" s="34" t="s">
+        <v>295</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="32" t="s">
+        <v>415</v>
+      </c>
+      <c r="B108" s="2"/>
+      <c r="D108" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="32" t="s">
+        <v>416</v>
+      </c>
+      <c r="B109" s="2"/>
+      <c r="D109" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="32" t="s">
+        <v>417</v>
+      </c>
+      <c r="B110" s="2"/>
+      <c r="D110" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="32" t="s">
+        <v>418</v>
+      </c>
+      <c r="B111" s="2"/>
+      <c r="D111" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="B112" s="2"/>
+      <c r="D112" s="34"/>
+      <c r="E112" s="9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="32"/>
+      <c r="B113" s="2"/>
+      <c r="E113" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="B114" s="2"/>
+      <c r="D114" s="34" t="s">
+        <v>300</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="32"/>
+      <c r="B115" s="2"/>
+      <c r="D115" s="34" t="s">
+        <v>301</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="32" t="s">
+        <v>411</v>
+      </c>
+      <c r="B116" s="2"/>
+      <c r="D116" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="E116" s="9" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="32" t="s">
+        <v>420</v>
+      </c>
+      <c r="B117" s="2"/>
+      <c r="D117" s="34" t="s">
+        <v>306</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="32"/>
+      <c r="B118" s="2"/>
+      <c r="D118" s="34"/>
+      <c r="E118" s="9" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="32" t="s">
+        <v>421</v>
+      </c>
+      <c r="B119" s="2"/>
+      <c r="D119" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="E119" s="9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="32" t="s">
+        <v>423</v>
+      </c>
+      <c r="B120" s="2"/>
+      <c r="D120" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="E120" s="9" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="32" t="s">
+        <v>423</v>
+      </c>
+      <c r="B121" s="2"/>
+      <c r="D121" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="E121" s="9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="32" t="s">
+        <v>422</v>
+      </c>
+      <c r="B122" s="2"/>
+      <c r="D122" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="32"/>
+      <c r="B123" s="2"/>
+      <c r="D123" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="E123" s="9" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="32"/>
+      <c r="B124" s="2"/>
+      <c r="D124" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="E124" s="9" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="32"/>
+      <c r="B125" s="2"/>
+      <c r="D125" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="E125" s="9" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="32"/>
+      <c r="B126" s="2"/>
+      <c r="D126" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="E126" s="9" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="32"/>
+      <c r="B127" s="2"/>
+      <c r="D127" s="34" t="s">
+        <v>326</v>
+      </c>
+      <c r="E127" s="9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="32"/>
+      <c r="B128" s="2"/>
+      <c r="D128" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="E128" s="9" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="32" t="s">
+        <v>424</v>
+      </c>
+      <c r="B129" s="2"/>
+      <c r="D129" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="E129" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="32" t="s">
+        <v>425</v>
+      </c>
+      <c r="B130" s="2"/>
+      <c r="D130" s="34"/>
+      <c r="E130" s="9" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="32" t="s">
+        <v>420</v>
+      </c>
+      <c r="B131" s="2"/>
+      <c r="D131" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="E131" s="9" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="32"/>
+      <c r="B132" s="2"/>
+      <c r="E132" s="9" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="32"/>
+      <c r="B133" s="2"/>
+      <c r="D133" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="E133" s="9" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="32"/>
+      <c r="B134" s="2"/>
+      <c r="D134" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="E134" s="9" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="32" t="s">
+        <v>426</v>
+      </c>
+      <c r="B135" s="2"/>
+      <c r="D135" s="34" t="s">
+        <v>339</v>
+      </c>
+      <c r="E135" s="9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="32" t="s">
+        <v>427</v>
+      </c>
+      <c r="B136" s="2"/>
+      <c r="D136" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="E136" s="9" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="32" t="s">
+        <v>428</v>
+      </c>
+      <c r="B137" s="2"/>
+      <c r="D137" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="E137" s="9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="32"/>
+      <c r="B138" s="2"/>
+      <c r="D138" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="E138" s="9" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="32"/>
+      <c r="B139" s="2"/>
+      <c r="D139" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="E139" s="9" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="32" t="s">
+        <v>420</v>
+      </c>
+      <c r="B140" s="2"/>
+      <c r="D140" s="34" t="s">
+        <v>350</v>
+      </c>
+      <c r="E140" s="9" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="29"/>
+      <c r="B141" s="2"/>
+      <c r="C141" s="32"/>
+      <c r="E141" s="9" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="29"/>
+      <c r="B142" s="2"/>
+      <c r="C142" s="32"/>
+      <c r="D142" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="E142" s="9" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="29"/>
+      <c r="B143" s="2"/>
+      <c r="C143" s="32"/>
+      <c r="D143" s="34" t="s">
+        <v>352</v>
+      </c>
+      <c r="E143" s="9" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="29"/>
+      <c r="B144" s="2"/>
+      <c r="C144" s="32"/>
+      <c r="D144" s="34"/>
+      <c r="E144" s="9"/>
+    </row>
+    <row r="145" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="29"/>
+      <c r="B145" s="2"/>
+      <c r="C145" s="32"/>
+      <c r="D145" s="34"/>
+      <c r="E145" s="9"/>
+    </row>
+    <row r="146" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="29"/>
+      <c r="B146" s="2"/>
+      <c r="C146" s="32"/>
+      <c r="D146" s="34"/>
+      <c r="E146" s="9"/>
+    </row>
+    <row r="147" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="29"/>
+      <c r="B147" s="2"/>
+      <c r="C147" s="32"/>
+      <c r="D147" s="34"/>
+      <c r="E147" s="9"/>
+    </row>
+    <row r="148" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="29"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="32"/>
+      <c r="D148" s="34"/>
+      <c r="E148" s="9"/>
+    </row>
+    <row r="149" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="29"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="32"/>
+      <c r="D149" s="34"/>
+      <c r="E149" s="9"/>
+    </row>
+    <row r="150" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="29"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="32"/>
+      <c r="D150" s="34"/>
+      <c r="E150" s="9"/>
+    </row>
+    <row r="151" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="29"/>
+      <c r="B151" s="2"/>
+      <c r="C151" s="32"/>
+      <c r="D151" s="34"/>
+      <c r="E151" s="9"/>
+    </row>
+    <row r="152" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="29"/>
+      <c r="B152" s="2"/>
+      <c r="C152" s="32"/>
+      <c r="D152" s="34"/>
+      <c r="E152" s="9"/>
+    </row>
+    <row r="153" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="29"/>
+      <c r="B153" s="2"/>
+      <c r="C153" s="32"/>
+      <c r="D153" s="34"/>
+      <c r="E153" s="9"/>
+    </row>
+    <row r="154" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="29"/>
+      <c r="B154" s="2"/>
+      <c r="C154" s="32"/>
+      <c r="D154" s="34"/>
+      <c r="E154" s="9"/>
+    </row>
+    <row r="155" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="29"/>
+      <c r="B155" s="2"/>
+      <c r="C155" s="32"/>
+      <c r="D155" s="34"/>
+      <c r="E155" s="9"/>
+    </row>
+    <row r="156" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="29"/>
+      <c r="B156" s="2"/>
+      <c r="C156" s="32"/>
+      <c r="D156" s="34"/>
+      <c r="E156" s="9"/>
+    </row>
+    <row r="157" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="29"/>
+      <c r="B157" s="2"/>
+      <c r="C157" s="32"/>
+      <c r="D157" s="34"/>
+      <c r="E157" s="9"/>
+    </row>
+    <row r="158" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="29"/>
+      <c r="B158" s="2"/>
+      <c r="C158" s="32"/>
+      <c r="D158" s="34"/>
+      <c r="E158" s="9"/>
+    </row>
+    <row r="159" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="29"/>
+      <c r="B159" s="2"/>
+      <c r="C159" s="32"/>
+      <c r="D159" s="34"/>
+      <c r="E159" s="9"/>
+    </row>
+    <row r="160" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="29"/>
+      <c r="B160" s="2"/>
+      <c r="C160" s="32"/>
+      <c r="D160" s="34"/>
+      <c r="E160" s="9"/>
+    </row>
+    <row r="161" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="29"/>
+      <c r="B161" s="2"/>
+      <c r="C161" s="32"/>
+      <c r="D161" s="34"/>
+      <c r="E161" s="9"/>
+    </row>
+    <row r="162" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="29"/>
+      <c r="B162" s="2"/>
+      <c r="C162" s="32"/>
+      <c r="D162" s="34"/>
+      <c r="E162" s="9"/>
+    </row>
+    <row r="163" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="29"/>
+      <c r="B163" s="2"/>
+      <c r="C163" s="32"/>
+      <c r="D163" s="34"/>
+      <c r="E163" s="9"/>
+    </row>
+    <row r="164" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="29"/>
+      <c r="B164" s="2"/>
+      <c r="C164" s="32"/>
+      <c r="D164" s="34"/>
+      <c r="E164" s="9"/>
+    </row>
+    <row r="165" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="29"/>
+      <c r="B165" s="2"/>
+      <c r="C165" s="32"/>
+      <c r="D165" s="34"/>
+      <c r="E165" s="9"/>
+    </row>
+    <row r="166" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="29"/>
+      <c r="B166" s="2"/>
+      <c r="C166" s="32"/>
+      <c r="D166" s="34"/>
+      <c r="E166" s="9"/>
+    </row>
+    <row r="167" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="29"/>
+      <c r="B167" s="2"/>
+      <c r="C167" s="32"/>
+      <c r="D167" s="34"/>
+      <c r="E167" s="9"/>
+    </row>
+    <row r="168" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="29"/>
+      <c r="B168" s="2"/>
+      <c r="C168" s="32"/>
+      <c r="D168" s="34"/>
+      <c r="E168" s="9"/>
+    </row>
+    <row r="169" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="29"/>
+      <c r="B169" s="2"/>
+      <c r="C169" s="32"/>
+      <c r="D169" s="34"/>
+      <c r="E169" s="9"/>
+    </row>
+    <row r="170" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="29"/>
+      <c r="B170" s="2"/>
+      <c r="C170" s="32"/>
+      <c r="D170" s="34"/>
+      <c r="E170" s="9"/>
+    </row>
+    <row r="171" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="29"/>
+      <c r="B171" s="2"/>
+      <c r="C171" s="32"/>
+      <c r="D171" s="34"/>
+      <c r="E171" s="9"/>
+    </row>
+    <row r="172" spans="1:5" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="29"/>
+      <c r="B172" s="2"/>
+      <c r="C172" s="32"/>
+      <c r="D172" s="34"/>
+      <c r="E172" s="9"/>
+    </row>
+    <row r="173" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A173" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="9" t="s">
+      <c r="B173" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C173" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E173" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="174" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A174" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="B174" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C174" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="D174" s="3"/>
+      <c r="E174" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="175" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A175" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="B175" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D175" s="3"/>
+      <c r="E175" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D176" s="20"/>
+      <c r="E176" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" ht="56" x14ac:dyDescent="0.2">
+      <c r="A177" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D177" s="3"/>
+      <c r="E177" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B178" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D178" s="3"/>
+      <c r="E178" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" s="16" customFormat="1" ht="67.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="22"/>
+      <c r="B179" s="22"/>
+      <c r="C179" s="7"/>
+      <c r="D179" s="7"/>
+      <c r="E179" s="8"/>
+    </row>
+    <row r="180" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A180" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C180" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="10" t="s">
+      <c r="D180" s="3"/>
+      <c r="E180" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" ht="65.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D181" s="3"/>
+      <c r="E181" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" ht="56" x14ac:dyDescent="0.2">
+      <c r="A182" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D182" s="3"/>
+      <c r="E182" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A183" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C183" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D183" s="17"/>
+      <c r="E183" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+      <c r="A184" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C184" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="56" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="16" customFormat="1" ht="67.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="65.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="56" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="9" t="s">
+      <c r="D184" s="3"/>
+      <c r="E184" s="2" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A179:B179"/>
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1249,116 +4041,116 @@
   <sheetData>
     <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="40.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>73</v>
-      </c>
       <c r="D2" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="13" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="13" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="27">
+      <c r="D4" s="21">
         <v>44786</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
     </row>
     <row r="8" spans="1:4" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25"/>
+      <c r="A8" s="19"/>
     </row>
     <row r="9" spans="1:4" ht="73.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="25"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
     </row>
     <row r="13" spans="1:4" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="20"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="20"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="25"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="17"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1367,6 +4159,93 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Funding_x0020_Source xmlns="d55fe6c3-41eb-40d5-bf17-87828c6d549e">110</Funding_x0020_Source>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef5a8d25-ade4-4894-b586-bac44eebb87b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <ATS_x0020_ID xmlns="d55fe6c3-41eb-40d5-bf17-87828c6d549e" xsi:nil="true"/>
+    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Document_x0020_Purpose xmlns="ef5a8d25-ade4-4894-b586-bac44eebb87b" xsi:nil="true"/>
+    <Route_x0020_To xmlns="ef5a8d25-ade4-4894-b586-bac44eebb87b">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </Route_x0020_To>
+    <TaxCatchAll xmlns="d55fe6c3-41eb-40d5-bf17-87828c6d549e" xsi:nil="true"/>
+    <External_x0020_Document xmlns="ef5a8d25-ade4-4894-b586-bac44eebb87b">false</External_x0020_Document>
+    <_dlc_DocId xmlns="d55fe6c3-41eb-40d5-bf17-87828c6d549e">5YHASYYS6FED-1857057342-19394</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="d55fe6c3-41eb-40d5-bf17-87828c6d549e">
+      <Url>https://sgi1.sharepoint.com/_layouts/15/DocIdRedir.aspx?ID=5YHASYYS6FED-1857057342-19394</Url>
+      <Description>5YHASYYS6FED-1857057342-19394</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086C757EFC63CB7438E4FDF6BDA8CEEFD" ma:contentTypeVersion="43" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ddd7f1a2ed0a147750bf6b134aff7355">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ef5a8d25-ade4-4894-b586-bac44eebb87b" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns4="d55fe6c3-41eb-40d5-bf17-87828c6d549e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e06d8c4cb20204d9966e87a30c98b86" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="ef5a8d25-ade4-4894-b586-bac44eebb87b"/>
@@ -1768,94 +4647,41 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Funding_x0020_Source xmlns="d55fe6c3-41eb-40d5-bf17-87828c6d549e">110</Funding_x0020_Source>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ef5a8d25-ade4-4894-b586-bac44eebb87b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <ATS_x0020_ID xmlns="d55fe6c3-41eb-40d5-bf17-87828c6d549e" xsi:nil="true"/>
-    <_Status xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Document_x0020_Purpose xmlns="ef5a8d25-ade4-4894-b586-bac44eebb87b" xsi:nil="true"/>
-    <Route_x0020_To xmlns="ef5a8d25-ade4-4894-b586-bac44eebb87b">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </Route_x0020_To>
-    <TaxCatchAll xmlns="d55fe6c3-41eb-40d5-bf17-87828c6d549e" xsi:nil="true"/>
-    <External_x0020_Document xmlns="ef5a8d25-ade4-4894-b586-bac44eebb87b">false</External_x0020_Document>
-    <_dlc_DocId xmlns="d55fe6c3-41eb-40d5-bf17-87828c6d549e">5YHASYYS6FED-1857057342-19394</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="d55fe6c3-41eb-40d5-bf17-87828c6d549e">
-      <Url>https://sgi1.sharepoint.com/_layouts/15/DocIdRedir.aspx?ID=5YHASYYS6FED-1857057342-19394</Url>
-      <Description>5YHASYYS6FED-1857057342-19394</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDE609AF-5E20-46AA-B1A6-01C0EC03D6CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3566766-E29D-4653-AA24-02A8145A2700}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31DB081F-618E-4837-B4E1-6FBC0F6A6583}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="d55fe6c3-41eb-40d5-bf17-87828c6d549e"/>
+    <ds:schemaRef ds:uri="ef5a8d25-ade4-4894-b586-bac44eebb87b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84BA7DBD-224F-4063-AE89-B2D5B6789011}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1873,38 +4699,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31DB081F-618E-4837-B4E1-6FBC0F6A6583}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="d55fe6c3-41eb-40d5-bf17-87828c6d549e"/>
-    <ds:schemaRef ds:uri="ef5a8d25-ade4-4894-b586-bac44eebb87b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3566766-E29D-4653-AA24-02A8145A2700}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDE609AF-5E20-46AA-B1A6-01C0EC03D6CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>